<commit_message>
fixed labels for 'CFA d7NS'
</commit_message>
<xml_diff>
--- a/Data/in/input.xlsx
+++ b/Data/in/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Repositories\gini\Data\in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acuna\Documents\Gini\Data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B68CBD-3F1A-4EB9-BED2-2E05ACA5F11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7F0352-372F-44A6-931E-861F35DDECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="268">
   <si>
     <t>Saline d1</t>
   </si>
@@ -841,9 +841,6 @@
   </si>
   <si>
     <t>t52</t>
-  </si>
-  <si>
-    <t>CFA d7 NS</t>
   </si>
 </sst>
 </file>
@@ -1349,42 +1346,42 @@
   <dimension ref="A1:AF226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI184" sqref="AI176:AI184"/>
+      <selection activeCell="N220" sqref="N220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="14" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" customWidth="1"/>
-    <col min="16" max="17" width="8.109375" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="13" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" customWidth="1"/>
+    <col min="16" max="17" width="8.140625" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="25" width="12.44140625" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="24" max="25" width="12.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" customWidth="1"/>
-    <col min="29" max="29" width="8.6640625" customWidth="1"/>
-    <col min="30" max="30" width="5.6640625" customWidth="1"/>
-    <col min="31" max="31" width="11.6640625" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="8.7109375" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" customWidth="1"/>
+    <col min="31" max="31" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1482,7 +1479,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>50</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>4.2187999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>50</v>
       </c>
@@ -1678,7 +1675,7 @@
         <v>3.1875</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>51</v>
       </c>
@@ -1776,7 +1773,7 @@
         <v>1.1561999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1872,7 +1869,7 @@
         <v>3.5937999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1968,7 +1965,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="7" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>53</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2162,7 +2159,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2260,7 +2257,7 @@
         <v>2.2187999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>54</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>54</v>
       </c>
@@ -2456,7 +2453,7 @@
         <v>4.1875</v>
       </c>
     </row>
-    <row r="12" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>54</v>
       </c>
@@ -2552,7 +2549,7 @@
         <v>6.125</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2650,7 +2647,7 @@
         <v>2.9687999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2748,7 +2745,7 @@
         <v>4.3849999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2844,7 +2841,7 @@
         <v>4.4974999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2942,7 +2939,7 @@
         <v>4.1562000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -3040,7 +3037,7 @@
         <v>3.0312000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3138,7 +3135,7 @@
         <v>2.8125</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3234,7 +3231,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3330,7 +3327,7 @@
         <v>8.9687999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>56</v>
       </c>
@@ -3428,7 +3425,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>56</v>
       </c>
@@ -3520,7 +3517,7 @@
         <v>8.5937999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>56</v>
       </c>
@@ -3618,7 +3615,7 @@
         <v>5.1562000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>56</v>
       </c>
@@ -3714,7 +3711,7 @@
         <v>9.875</v>
       </c>
     </row>
-    <row r="25" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>56</v>
       </c>
@@ -3812,7 +3809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>56</v>
       </c>
@@ -3910,7 +3907,7 @@
         <v>4.625</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4008,7 +4005,7 @@
         <v>4.8437999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -4106,7 +4103,7 @@
         <v>5.8437999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -4198,7 +4195,7 @@
         <v>2.6562000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -4291,7 +4288,7 @@
         <v>1.5938000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -4389,7 +4386,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -4487,7 +4484,7 @@
         <v>7.6875</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -4585,7 +4582,7 @@
         <v>11.406000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -4681,7 +4678,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -4779,7 +4776,7 @@
         <v>3.6562000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -4877,7 +4874,7 @@
         <v>5.6562000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -4975,7 +4972,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -5073,7 +5070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -5171,7 +5168,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -5269,7 +5266,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -5367,7 +5364,7 @@
         <v>1.4375</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -5463,7 +5460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -5561,7 +5558,7 @@
         <v>1.385</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -5657,7 +5654,7 @@
         <v>4.8437999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -5752,7 +5749,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -5847,7 +5844,7 @@
         <v>3.2812000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -5942,7 +5939,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -6035,7 +6032,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -6128,7 +6125,7 @@
         <v>7.4062000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -6223,7 +6220,7 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -6318,7 +6315,7 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -6413,7 +6410,7 @@
         <v>6.1875</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -6506,7 +6503,7 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -6601,7 +6598,7 @@
         <v>1.5625</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -6690,7 +6687,7 @@
         <v>7.5937999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -6788,7 +6785,7 @@
         <v>8.4687999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -6883,7 +6880,7 @@
         <v>3.0625</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -6978,7 +6975,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -7073,7 +7070,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -7168,7 +7165,7 @@
         <v>2.3437999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -7263,7 +7260,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -7358,7 +7355,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -7453,7 +7450,7 @@
         <v>8.4062000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -7548,7 +7545,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -7643,7 +7640,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -7736,7 +7733,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -7831,7 +7828,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -7926,7 +7923,7 @@
         <v>2.1875</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -8022,7 +8019,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -8115,7 +8112,7 @@
         <v>6.9062000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -8210,7 +8207,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -8303,7 +8300,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -8399,7 +8396,7 @@
         <v>2.4062000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -8497,7 +8494,7 @@
         <v>1.9688000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -8592,7 +8589,7 @@
         <v>3.0312000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -8687,7 +8684,7 @@
         <v>1.0938000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -8780,7 +8777,7 @@
         <v>6.5625</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -8875,7 +8872,7 @@
         <v>1.0311999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -8964,7 +8961,7 @@
         <v>0.96875</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -9059,7 +9056,7 @@
         <v>2.0937999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -9154,7 +9151,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -9249,7 +9246,7 @@
         <v>1.7188000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -9344,7 +9341,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -9439,7 +9436,7 @@
         <v>-1.8125</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -9532,7 +9529,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -9627,7 +9624,7 @@
         <v>1.6875</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -9722,7 +9719,7 @@
         <v>5.0312000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -9817,7 +9814,7 @@
         <v>4.4687999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -9912,7 +9909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -10007,7 +10004,7 @@
         <v>2.4375</v>
       </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -10102,7 +10099,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -10197,7 +10194,7 @@
         <v>1.0625</v>
       </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -10292,7 +10289,7 @@
         <v>4.9687999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>86</v>
       </c>
@@ -10387,7 +10384,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -10480,7 +10477,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -10566,7 +10563,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -10661,7 +10658,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>89</v>
       </c>
@@ -10750,7 +10747,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -10845,7 +10842,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>90</v>
       </c>
@@ -10940,7 +10937,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>90</v>
       </c>
@@ -11035,7 +11032,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -11130,7 +11127,7 @@
         <v>3.0625</v>
       </c>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -11225,7 +11222,7 @@
         <v>1.7188000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -11320,7 +11317,7 @@
         <v>13.688000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -11413,7 +11410,7 @@
         <v>2.4375</v>
       </c>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -11508,7 +11505,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>94</v>
       </c>
@@ -11603,7 +11600,7 @@
         <v>2.2812000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>95</v>
       </c>
@@ -11698,7 +11695,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>96</v>
       </c>
@@ -11793,7 +11790,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -11888,7 +11885,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -11983,7 +11980,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -12078,7 +12075,7 @@
         <v>3.4062000000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>98</v>
       </c>
@@ -12173,7 +12170,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>98</v>
       </c>
@@ -12268,7 +12265,7 @@
         <v>1.9061999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -12363,7 +12360,7 @@
         <v>2.6274999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>30</v>
       </c>
@@ -12458,7 +12455,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -12553,7 +12550,7 @@
         <v>3.6562000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>29</v>
       </c>
@@ -12648,7 +12645,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="119" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22" t="s">
         <v>30</v>
       </c>
@@ -12743,7 +12740,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="120" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22" t="s">
         <v>29</v>
       </c>
@@ -12838,7 +12835,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="121" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="22" t="s">
         <v>29</v>
       </c>
@@ -12933,7 +12930,7 @@
         <v>3.1562000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="22" t="s">
         <v>29</v>
       </c>
@@ -13028,7 +13025,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="123" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
         <v>29</v>
       </c>
@@ -13123,7 +13120,7 @@
         <v>2.9687999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
         <v>29</v>
       </c>
@@ -13218,7 +13215,7 @@
         <v>4.8125</v>
       </c>
     </row>
-    <row r="125" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
         <v>29</v>
       </c>
@@ -13313,7 +13310,7 @@
         <v>3.8437999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
         <v>29</v>
       </c>
@@ -13408,7 +13405,7 @@
         <v>10.906000000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>29</v>
       </c>
@@ -13503,7 +13500,7 @@
         <v>3.3437999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="22" t="s">
         <v>29</v>
       </c>
@@ -13598,7 +13595,7 @@
         <v>3.6875</v>
       </c>
     </row>
-    <row r="129" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="22" t="s">
         <v>29</v>
       </c>
@@ -13693,7 +13690,7 @@
         <v>11.093999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="22" t="s">
         <v>29</v>
       </c>
@@ -13788,7 +13785,7 @@
         <v>5.5937999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="22" t="s">
         <v>30</v>
       </c>
@@ -13883,7 +13880,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="22" t="s">
         <v>30</v>
       </c>
@@ -13978,7 +13975,7 @@
         <v>-6.25E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="22" t="s">
         <v>29</v>
       </c>
@@ -14073,7 +14070,7 @@
         <v>6.0937999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="22" t="s">
         <v>30</v>
       </c>
@@ -14168,7 +14165,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="135" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="22" t="s">
         <v>30</v>
       </c>
@@ -14263,7 +14260,7 @@
         <v>1.0311999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="22" t="s">
         <v>29</v>
       </c>
@@ -14358,7 +14355,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="22" t="s">
         <v>29</v>
       </c>
@@ -14453,7 +14450,7 @@
         <v>6.125</v>
       </c>
     </row>
-    <row r="138" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="22" t="s">
         <v>29</v>
       </c>
@@ -14548,7 +14545,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="22" t="s">
         <v>30</v>
       </c>
@@ -14643,7 +14640,7 @@
         <v>1.6561999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="22" t="s">
         <v>29</v>
       </c>
@@ -14738,7 +14735,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="141" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="22" t="s">
         <v>29</v>
       </c>
@@ -14833,7 +14830,7 @@
         <v>4.5625</v>
       </c>
     </row>
-    <row r="142" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="22" t="s">
         <v>29</v>
       </c>
@@ -14910,7 +14907,7 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>29</v>
       </c>
@@ -15005,7 +15002,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -15100,7 +15097,7 @@
         <v>3.1562000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>29</v>
       </c>
@@ -15195,7 +15192,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>29</v>
       </c>
@@ -15290,7 +15287,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>49</v>
       </c>
@@ -15388,7 +15385,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>29</v>
       </c>
@@ -15438,7 +15435,7 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>30818</v>
       </c>
@@ -15485,7 +15482,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>30818</v>
       </c>
@@ -15532,7 +15529,7 @@
         <v>4.6562000000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>30818</v>
       </c>
@@ -15579,7 +15576,7 @@
         <v>4.9687999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>30818</v>
       </c>
@@ -15626,7 +15623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>30818</v>
       </c>
@@ -15673,7 +15670,7 @@
         <v>4.0937999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>30818</v>
       </c>
@@ -15718,7 +15715,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>30818</v>
       </c>
@@ -15765,7 +15762,7 @@
         <v>2.1562000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>30818</v>
       </c>
@@ -15812,7 +15809,7 @@
         <v>2.6875</v>
       </c>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>30818</v>
       </c>
@@ -15856,7 +15853,7 @@
         <v>-0.28125</v>
       </c>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>60818</v>
       </c>
@@ -15903,7 +15900,7 @@
         <v>6.9062000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>60818</v>
       </c>
@@ -15950,7 +15947,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>60818</v>
       </c>
@@ -15997,10 +15994,10 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="161" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:32" x14ac:dyDescent="0.25">
       <c r="E161" s="22"/>
     </row>
-    <row r="162" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>60818</v>
       </c>
@@ -16047,7 +16044,7 @@
         <v>9.0937999999999999</v>
       </c>
     </row>
-    <row r="163" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>60818</v>
       </c>
@@ -16094,7 +16091,7 @@
         <v>5.0937999999999999</v>
       </c>
     </row>
-    <row r="164" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>60818</v>
       </c>
@@ -16141,7 +16138,7 @@
         <v>0.96850000000000003</v>
       </c>
     </row>
-    <row r="165" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>60818</v>
       </c>
@@ -16188,7 +16185,7 @@
         <v>3.5312000000000001</v>
       </c>
     </row>
-    <row r="166" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>70818</v>
       </c>
@@ -16235,7 +16232,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="167" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>70818</v>
       </c>
@@ -16282,7 +16279,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="168" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>70818</v>
       </c>
@@ -16329,7 +16326,7 @@
         <v>2.7812000000000001</v>
       </c>
     </row>
-    <row r="169" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>70818</v>
       </c>
@@ -16376,7 +16373,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="170" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>70818</v>
       </c>
@@ -16423,7 +16420,7 @@
         <v>2.1850000000000001</v>
       </c>
     </row>
-    <row r="171" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>70818</v>
       </c>
@@ -16470,7 +16467,7 @@
         <v>3.7187999999999999</v>
       </c>
     </row>
-    <row r="172" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>70818</v>
       </c>
@@ -16514,7 +16511,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="173" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>70818</v>
       </c>
@@ -16561,7 +16558,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="174" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>70818</v>
       </c>
@@ -16608,7 +16605,7 @@
         <v>9.3125</v>
       </c>
     </row>
-    <row r="175" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>140818</v>
       </c>
@@ -16652,7 +16649,7 @@
         <v>3.9687999999999999</v>
       </c>
     </row>
-    <row r="176" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>140818</v>
       </c>
@@ -16699,7 +16696,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="177" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>140818</v>
       </c>
@@ -16746,7 +16743,7 @@
         <v>5.7187999999999999</v>
       </c>
     </row>
-    <row r="178" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>140818</v>
       </c>
@@ -16793,7 +16790,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="179" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>140818</v>
       </c>
@@ -16837,7 +16834,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="180" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>140818</v>
       </c>
@@ -16881,7 +16878,7 @@
         <v>1.4061999999999999</v>
       </c>
     </row>
-    <row r="181" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>300518</v>
       </c>
@@ -16928,7 +16925,7 @@
         <v>4.1875</v>
       </c>
     </row>
-    <row r="182" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>300518</v>
       </c>
@@ -16975,7 +16972,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="183" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>300518</v>
       </c>
@@ -17022,7 +17019,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="184" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>300518</v>
       </c>
@@ -17069,7 +17066,7 @@
         <v>1.4337500000000001</v>
       </c>
     </row>
-    <row r="185" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>300518</v>
       </c>
@@ -17116,7 +17113,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="186" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>300518</v>
       </c>
@@ -17163,7 +17160,7 @@
         <v>3.5937999999999999</v>
       </c>
     </row>
-    <row r="187" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>300518</v>
       </c>
@@ -17210,7 +17207,7 @@
         <v>3.2812000000000001</v>
       </c>
     </row>
-    <row r="188" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>300518</v>
       </c>
@@ -17255,7 +17252,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="189" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>70618</v>
       </c>
@@ -17302,7 +17299,7 @@
         <v>-1.0311999999999999</v>
       </c>
     </row>
-    <row r="190" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>70618</v>
       </c>
@@ -17349,7 +17346,7 @@
         <v>3.7187999999999999</v>
       </c>
     </row>
-    <row r="191" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>70618</v>
       </c>
@@ -17396,7 +17393,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="192" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>70618</v>
       </c>
@@ -17443,7 +17440,7 @@
         <v>2.6440000000000001</v>
       </c>
     </row>
-    <row r="193" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>70618</v>
       </c>
@@ -17490,7 +17487,7 @@
         <v>5.1562000000000001</v>
       </c>
     </row>
-    <row r="194" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>70618</v>
       </c>
@@ -17537,7 +17534,7 @@
         <v>2.0937999999999999</v>
       </c>
     </row>
-    <row r="195" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>70618</v>
       </c>
@@ -17584,7 +17581,7 @@
         <v>3.5312000000000001</v>
       </c>
     </row>
-    <row r="196" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>70618</v>
       </c>
@@ -17631,7 +17628,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="197" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>70618</v>
       </c>
@@ -17678,7 +17675,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="198" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>70618</v>
       </c>
@@ -17725,7 +17722,7 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="199" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>70618</v>
       </c>
@@ -17772,7 +17769,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="200" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>80618</v>
       </c>
@@ -17819,7 +17816,7 @@
         <v>2.7187999999999999</v>
       </c>
     </row>
-    <row r="201" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>80618</v>
       </c>
@@ -17866,7 +17863,7 @@
         <v>3.9687999999999999</v>
       </c>
     </row>
-    <row r="202" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>80618</v>
       </c>
@@ -17913,7 +17910,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="203" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B203">
         <v>80618</v>
       </c>
@@ -17960,7 +17957,7 @@
         <v>2.5937999999999999</v>
       </c>
     </row>
-    <row r="204" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B204">
         <v>80618</v>
       </c>
@@ -18007,7 +18004,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="205" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B205">
         <v>80618</v>
       </c>
@@ -18054,7 +18051,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="206" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>251018</v>
       </c>
@@ -18101,7 +18098,7 @@
         <v>4.2187999999999999</v>
       </c>
     </row>
-    <row r="207" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>251018</v>
       </c>
@@ -18148,7 +18145,7 @@
         <v>2.0312000000000001</v>
       </c>
     </row>
-    <row r="208" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>251018</v>
       </c>
@@ -18195,7 +18192,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="209" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>261018</v>
       </c>
@@ -18242,7 +18239,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="210" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>261018</v>
       </c>
@@ -18289,7 +18286,7 @@
         <v>3.4062000000000001</v>
       </c>
     </row>
-    <row r="211" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>261018</v>
       </c>
@@ -18336,7 +18333,7 @@
         <v>3.6875</v>
       </c>
     </row>
-    <row r="212" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>261018</v>
       </c>
@@ -18380,7 +18377,7 @@
         <v>9.4062000000000001</v>
       </c>
     </row>
-    <row r="213" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>220519</v>
       </c>
@@ -18427,7 +18424,7 @@
         <v>8.6861999999999995</v>
       </c>
     </row>
-    <row r="214" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>220519</v>
       </c>
@@ -18471,7 +18468,7 @@
         <v>4.0620000000000003</v>
       </c>
     </row>
-    <row r="215" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>220519</v>
       </c>
@@ -18518,7 +18515,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="216" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B216">
         <v>220519</v>
       </c>
@@ -18565,7 +18562,7 @@
         <v>5.1875</v>
       </c>
     </row>
-    <row r="217" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B217">
         <v>40918</v>
       </c>
@@ -18609,7 +18606,7 @@
         <v>4.5320999999999998</v>
       </c>
     </row>
-    <row r="218" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B218">
         <v>40918</v>
       </c>
@@ -18653,12 +18650,12 @@
         <v>3.3125</v>
       </c>
     </row>
-    <row r="219" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B219">
         <v>11018</v>
       </c>
       <c r="C219" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="D219">
         <v>2</v>
@@ -18700,12 +18697,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B220">
         <v>11018</v>
       </c>
       <c r="C220" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="D220">
         <v>2</v>
@@ -18747,12 +18744,12 @@
         <v>5.9687999999999999</v>
       </c>
     </row>
-    <row r="221" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B221">
         <v>21018</v>
       </c>
       <c r="C221" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="D221">
         <v>2</v>
@@ -18791,12 +18788,12 @@
         <v>0.21875</v>
       </c>
     </row>
-    <row r="222" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B222">
         <v>21018</v>
       </c>
       <c r="C222" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="D222">
         <v>2</v>
@@ -18838,12 +18835,12 @@
         <v>1.1875</v>
       </c>
     </row>
-    <row r="223" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B223">
         <v>270319</v>
       </c>
       <c r="C223" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="E223" s="22" t="s">
         <v>28</v>
@@ -18883,12 +18880,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="224" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B224">
         <v>270319</v>
       </c>
       <c r="C224" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="E224" s="22" t="s">
         <v>47</v>
@@ -18927,12 +18924,12 @@
         <v>4.1224999999999996</v>
       </c>
     </row>
-    <row r="225" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B225">
         <v>270319</v>
       </c>
       <c r="C225" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="E225" s="22" t="s">
         <v>35</v>
@@ -18969,12 +18966,12 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="226" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B226">
         <v>270320</v>
       </c>
       <c r="C226" t="s">
-        <v>268</v>
+        <v>107</v>
       </c>
       <c r="E226" s="22" t="s">
         <v>44</v>
@@ -19031,13 +19028,13 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
@@ -19056,7 +19053,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -19071,7 +19068,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
@@ -19090,7 +19087,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -19107,7 +19104,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -19120,7 +19117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>21</v>
       </c>
@@ -19139,7 +19136,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -19158,7 +19155,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -19177,7 +19174,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -19196,7 +19193,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -19215,7 +19212,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -19234,7 +19231,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
@@ -19255,7 +19252,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -19274,7 +19271,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K20" s="8" t="s">
         <v>16</v>
       </c>
@@ -19285,7 +19282,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -19299,43 +19296,43 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>

</xml_diff>

<commit_message>
Neurons added from Natalie reconstructions
</commit_message>
<xml_diff>
--- a/Data/in/input.xlsx
+++ b/Data/in/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acuna\Documents\Gini\Data\in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Repositories\gini\Data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7F0352-372F-44A6-931E-861F35DDECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2988EA3-A7BD-40A5-9E79-D573DD5E2D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="272">
   <si>
     <t>Saline d1</t>
   </si>
@@ -841,6 +841,18 @@
   </si>
   <si>
     <t>t52</t>
+  </si>
+  <si>
+    <t>DAP</t>
+  </si>
+  <si>
+    <t>ReboundD</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>L2/3</t>
   </si>
 </sst>
 </file>
@@ -870,7 +882,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,6 +892,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1029,6 +1047,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,43 +1364,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565C04A2-646C-44CE-A1DE-AE1439B22FF5}">
   <dimension ref="A1:AF226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N220" sqref="N220"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="4.7109375" customWidth="1"/>
-    <col min="16" max="17" width="8.140625" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="13" max="14" width="7.6640625" customWidth="1"/>
+    <col min="15" max="15" width="4.6640625" customWidth="1"/>
+    <col min="16" max="17" width="8.109375" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" customWidth="1"/>
-    <col min="22" max="22" width="8.85546875" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="24" max="25" width="12.42578125" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="25" width="12.44140625" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" customWidth="1"/>
-    <col min="30" max="30" width="5.7109375" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" customWidth="1"/>
+    <col min="30" max="30" width="5.6640625" customWidth="1"/>
+    <col min="31" max="31" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1467,7 +1486,7 @@
         <v>248</v>
       </c>
       <c r="AC1" s="16" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>250</v>
@@ -1476,10 +1495,10 @@
         <v>253</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>50</v>
       </c>
@@ -1577,7 +1596,7 @@
         <v>4.2187999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>50</v>
       </c>
@@ -1675,7 +1694,7 @@
         <v>3.1875</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>51</v>
       </c>
@@ -1773,7 +1792,7 @@
         <v>1.1561999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1869,7 +1888,7 @@
         <v>3.5937999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1965,7 +1984,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="7" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>53</v>
       </c>
@@ -2063,7 +2082,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2159,7 +2178,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2257,7 +2276,7 @@
         <v>2.2187999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>54</v>
       </c>
@@ -2355,7 +2374,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>54</v>
       </c>
@@ -2453,7 +2472,7 @@
         <v>4.1875</v>
       </c>
     </row>
-    <row r="12" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>54</v>
       </c>
@@ -2549,7 +2568,7 @@
         <v>6.125</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2647,7 +2666,7 @@
         <v>2.9687999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2745,7 +2764,7 @@
         <v>4.3849999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2841,7 +2860,7 @@
         <v>4.4974999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2939,7 +2958,7 @@
         <v>4.1562000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -3037,7 +3056,7 @@
         <v>3.0312000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3135,7 +3154,7 @@
         <v>2.8125</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3231,7 +3250,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3327,7 +3346,7 @@
         <v>8.9687999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>56</v>
       </c>
@@ -3425,7 +3444,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>56</v>
       </c>
@@ -3517,7 +3536,7 @@
         <v>8.5937999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>56</v>
       </c>
@@ -3615,7 +3634,7 @@
         <v>5.1562000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>56</v>
       </c>
@@ -3711,7 +3730,7 @@
         <v>9.875</v>
       </c>
     </row>
-    <row r="25" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>56</v>
       </c>
@@ -3809,7 +3828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>56</v>
       </c>
@@ -3907,7 +3926,7 @@
         <v>4.625</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4005,7 +4024,7 @@
         <v>4.8437999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -4103,7 +4122,7 @@
         <v>5.8437999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -4195,7 +4214,7 @@
         <v>2.6562000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -4288,7 +4307,7 @@
         <v>1.5938000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -4386,7 +4405,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -4484,7 +4503,7 @@
         <v>7.6875</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -4582,7 +4601,7 @@
         <v>11.406000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -4678,7 +4697,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -4776,7 +4795,7 @@
         <v>3.6562000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -4874,7 +4893,7 @@
         <v>5.6562000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -4972,7 +4991,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -5070,7 +5089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -5168,7 +5187,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -5266,7 +5285,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -5364,7 +5383,7 @@
         <v>1.4375</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -5460,7 +5479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -5558,7 +5577,7 @@
         <v>1.385</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -5654,7 +5673,7 @@
         <v>4.8437999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -5749,7 +5768,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -5844,7 +5863,7 @@
         <v>3.2812000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -5939,7 +5958,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -6032,7 +6051,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -6125,7 +6144,7 @@
         <v>7.4062000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -6220,7 +6239,7 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -6315,7 +6334,7 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -6410,7 +6429,7 @@
         <v>6.1875</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -6503,7 +6522,7 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -6598,7 +6617,7 @@
         <v>1.5625</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -6687,7 +6706,7 @@
         <v>7.5937999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -6785,7 +6804,7 @@
         <v>8.4687999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -6880,7 +6899,7 @@
         <v>3.0625</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -6975,7 +6994,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -7070,7 +7089,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -7165,7 +7184,7 @@
         <v>2.3437999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -7260,7 +7279,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -7355,7 +7374,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -7450,7 +7469,7 @@
         <v>8.4062000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -7545,7 +7564,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -7640,7 +7659,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -7733,7 +7752,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -7828,7 +7847,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -7923,7 +7942,7 @@
         <v>2.1875</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -8019,7 +8038,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -8112,7 +8131,7 @@
         <v>6.9062000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -8207,7 +8226,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -8300,7 +8319,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -8396,7 +8415,7 @@
         <v>2.4062000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -8494,7 +8513,7 @@
         <v>1.9688000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -8589,7 +8608,7 @@
         <v>3.0312000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -8684,7 +8703,7 @@
         <v>1.0938000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -8777,7 +8796,7 @@
         <v>6.5625</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -8872,7 +8891,7 @@
         <v>1.0311999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -8961,7 +8980,7 @@
         <v>0.96875</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -9056,7 +9075,7 @@
         <v>2.0937999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -9151,7 +9170,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -9246,7 +9265,7 @@
         <v>1.7188000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -9341,7 +9360,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -9436,7 +9455,7 @@
         <v>-1.8125</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -9529,7 +9548,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -9624,7 +9643,7 @@
         <v>1.6875</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -9719,7 +9738,7 @@
         <v>5.0312000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -9814,7 +9833,7 @@
         <v>4.4687999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -9909,7 +9928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -10004,7 +10023,7 @@
         <v>2.4375</v>
       </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -10099,7 +10118,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -10194,7 +10213,7 @@
         <v>1.0625</v>
       </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -10289,7 +10308,7 @@
         <v>4.9687999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>86</v>
       </c>
@@ -10384,7 +10403,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -10477,7 +10496,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -10563,7 +10582,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -10658,7 +10677,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>89</v>
       </c>
@@ -10747,7 +10766,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -10842,7 +10861,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>90</v>
       </c>
@@ -10937,7 +10956,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>90</v>
       </c>
@@ -11032,7 +11051,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -11127,7 +11146,7 @@
         <v>3.0625</v>
       </c>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -11222,7 +11241,7 @@
         <v>1.7188000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -11317,7 +11336,7 @@
         <v>13.688000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>93</v>
       </c>
@@ -11410,7 +11429,7 @@
         <v>2.4375</v>
       </c>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -11505,7 +11524,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>94</v>
       </c>
@@ -11600,7 +11619,7 @@
         <v>2.2812000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>95</v>
       </c>
@@ -11695,7 +11714,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>96</v>
       </c>
@@ -11790,7 +11809,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -11885,7 +11904,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -11980,7 +11999,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -12075,7 +12094,7 @@
         <v>3.4062000000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>98</v>
       </c>
@@ -12170,7 +12189,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>98</v>
       </c>
@@ -12265,7 +12284,7 @@
         <v>1.9061999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -12360,7 +12379,7 @@
         <v>2.6274999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>30</v>
       </c>
@@ -12455,7 +12474,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -12550,7 +12569,7 @@
         <v>3.6562000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>29</v>
       </c>
@@ -12645,7 +12664,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="119" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="22" t="s">
         <v>30</v>
       </c>
@@ -12740,7 +12759,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="120" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="22" t="s">
         <v>29</v>
       </c>
@@ -12835,7 +12854,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="121" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="22" t="s">
         <v>29</v>
       </c>
@@ -12930,7 +12949,7 @@
         <v>3.1562000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="22" t="s">
         <v>29</v>
       </c>
@@ -13025,7 +13044,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="123" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="22" t="s">
         <v>29</v>
       </c>
@@ -13120,7 +13139,7 @@
         <v>2.9687999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="22" t="s">
         <v>29</v>
       </c>
@@ -13215,7 +13234,7 @@
         <v>4.8125</v>
       </c>
     </row>
-    <row r="125" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="22" t="s">
         <v>29</v>
       </c>
@@ -13310,7 +13329,7 @@
         <v>3.8437999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
         <v>29</v>
       </c>
@@ -13405,7 +13424,7 @@
         <v>10.906000000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
         <v>29</v>
       </c>
@@ -13500,7 +13519,7 @@
         <v>3.3437999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
         <v>29</v>
       </c>
@@ -13595,7 +13614,7 @@
         <v>3.6875</v>
       </c>
     </row>
-    <row r="129" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
         <v>29</v>
       </c>
@@ -13690,7 +13709,7 @@
         <v>11.093999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="22" t="s">
         <v>29</v>
       </c>
@@ -13785,7 +13804,7 @@
         <v>5.5937999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="22" t="s">
         <v>30</v>
       </c>
@@ -13880,7 +13899,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="22" t="s">
         <v>30</v>
       </c>
@@ -13975,7 +13994,7 @@
         <v>-6.25E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="22" t="s">
         <v>29</v>
       </c>
@@ -14070,7 +14089,7 @@
         <v>6.0937999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
         <v>30</v>
       </c>
@@ -14165,7 +14184,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="135" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
         <v>30</v>
       </c>
@@ -14260,7 +14279,7 @@
         <v>1.0311999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="22" t="s">
         <v>29</v>
       </c>
@@ -14355,7 +14374,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
         <v>29</v>
       </c>
@@ -14450,7 +14469,7 @@
         <v>6.125</v>
       </c>
     </row>
-    <row r="138" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="22" t="s">
         <v>29</v>
       </c>
@@ -14545,7 +14564,7 @@
         <v>2.9062000000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="22" t="s">
         <v>30</v>
       </c>
@@ -14640,7 +14659,7 @@
         <v>1.6561999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="22" t="s">
         <v>29</v>
       </c>
@@ -14735,7 +14754,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="141" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="22" t="s">
         <v>29</v>
       </c>
@@ -14830,7 +14849,7 @@
         <v>4.5625</v>
       </c>
     </row>
-    <row r="142" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="22" t="s">
         <v>29</v>
       </c>
@@ -14907,7 +14926,7 @@
         <v>4.875</v>
       </c>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>29</v>
       </c>
@@ -15002,7 +15021,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -15097,7 +15116,7 @@
         <v>3.1562000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>29</v>
       </c>
@@ -15192,7 +15211,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>29</v>
       </c>
@@ -15287,7 +15306,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>49</v>
       </c>
@@ -15385,7 +15404,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>29</v>
       </c>
@@ -15435,7 +15454,7 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>30818</v>
       </c>
@@ -15482,7 +15501,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B150">
         <v>30818</v>
       </c>
@@ -15529,7 +15548,7 @@
         <v>4.6562000000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B151">
         <v>30818</v>
       </c>
@@ -15576,7 +15595,7 @@
         <v>4.9687999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B152">
         <v>30818</v>
       </c>
@@ -15623,7 +15642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B153">
         <v>30818</v>
       </c>
@@ -15670,7 +15689,7 @@
         <v>4.0937999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B154">
         <v>30818</v>
       </c>
@@ -15715,7 +15734,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B155">
         <v>30818</v>
       </c>
@@ -15762,7 +15781,7 @@
         <v>2.1562000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B156">
         <v>30818</v>
       </c>
@@ -15809,7 +15828,7 @@
         <v>2.6875</v>
       </c>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B157">
         <v>30818</v>
       </c>
@@ -15853,7 +15872,7 @@
         <v>-0.28125</v>
       </c>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B158">
         <v>60818</v>
       </c>
@@ -15900,7 +15919,7 @@
         <v>6.9062000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B159">
         <v>60818</v>
       </c>
@@ -15947,7 +15966,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B160">
         <v>60818</v>
       </c>
@@ -15994,10 +16013,10 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="161" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:32" x14ac:dyDescent="0.3">
       <c r="E161" s="22"/>
     </row>
-    <row r="162" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B162">
         <v>60818</v>
       </c>
@@ -16044,7 +16063,7 @@
         <v>9.0937999999999999</v>
       </c>
     </row>
-    <row r="163" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B163">
         <v>60818</v>
       </c>
@@ -16091,7 +16110,7 @@
         <v>5.0937999999999999</v>
       </c>
     </row>
-    <row r="164" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B164">
         <v>60818</v>
       </c>
@@ -16138,7 +16157,7 @@
         <v>0.96850000000000003</v>
       </c>
     </row>
-    <row r="165" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B165">
         <v>60818</v>
       </c>
@@ -16185,7 +16204,7 @@
         <v>3.5312000000000001</v>
       </c>
     </row>
-    <row r="166" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B166">
         <v>70818</v>
       </c>
@@ -16232,7 +16251,7 @@
         <v>1.8438000000000001</v>
       </c>
     </row>
-    <row r="167" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B167">
         <v>70818</v>
       </c>
@@ -16279,7 +16298,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="168" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B168">
         <v>70818</v>
       </c>
@@ -16326,7 +16345,7 @@
         <v>2.7812000000000001</v>
       </c>
     </row>
-    <row r="169" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B169">
         <v>70818</v>
       </c>
@@ -16373,7 +16392,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="170" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B170">
         <v>70818</v>
       </c>
@@ -16420,7 +16439,7 @@
         <v>2.1850000000000001</v>
       </c>
     </row>
-    <row r="171" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B171">
         <v>70818</v>
       </c>
@@ -16467,7 +16486,7 @@
         <v>3.7187999999999999</v>
       </c>
     </row>
-    <row r="172" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B172">
         <v>70818</v>
       </c>
@@ -16511,7 +16530,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="173" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B173">
         <v>70818</v>
       </c>
@@ -16558,7 +16577,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="174" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B174">
         <v>70818</v>
       </c>
@@ -16605,7 +16624,7 @@
         <v>9.3125</v>
       </c>
     </row>
-    <row r="175" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B175">
         <v>140818</v>
       </c>
@@ -16649,7 +16668,7 @@
         <v>3.9687999999999999</v>
       </c>
     </row>
-    <row r="176" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B176">
         <v>140818</v>
       </c>
@@ -16696,7 +16715,7 @@
         <v>3.4687999999999999</v>
       </c>
     </row>
-    <row r="177" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B177">
         <v>140818</v>
       </c>
@@ -16743,7 +16762,7 @@
         <v>5.7187999999999999</v>
       </c>
     </row>
-    <row r="178" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B178">
         <v>140818</v>
       </c>
@@ -16790,7 +16809,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="179" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B179">
         <v>140818</v>
       </c>
@@ -16834,7 +16853,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="180" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B180">
         <v>140818</v>
       </c>
@@ -16878,7 +16897,7 @@
         <v>1.4061999999999999</v>
       </c>
     </row>
-    <row r="181" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B181">
         <v>300518</v>
       </c>
@@ -16925,7 +16944,7 @@
         <v>4.1875</v>
       </c>
     </row>
-    <row r="182" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B182">
         <v>300518</v>
       </c>
@@ -16972,7 +16991,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="183" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B183">
         <v>300518</v>
       </c>
@@ -17019,7 +17038,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="184" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B184">
         <v>300518</v>
       </c>
@@ -17066,7 +17085,7 @@
         <v>1.4337500000000001</v>
       </c>
     </row>
-    <row r="185" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B185">
         <v>300518</v>
       </c>
@@ -17113,7 +17132,7 @@
         <v>2.5625</v>
       </c>
     </row>
-    <row r="186" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B186">
         <v>300518</v>
       </c>
@@ -17160,7 +17179,7 @@
         <v>3.5937999999999999</v>
       </c>
     </row>
-    <row r="187" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B187">
         <v>300518</v>
       </c>
@@ -17207,7 +17226,7 @@
         <v>3.2812000000000001</v>
       </c>
     </row>
-    <row r="188" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B188">
         <v>300518</v>
       </c>
@@ -17252,7 +17271,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="189" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B189">
         <v>70618</v>
       </c>
@@ -17299,7 +17318,7 @@
         <v>-1.0311999999999999</v>
       </c>
     </row>
-    <row r="190" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B190">
         <v>70618</v>
       </c>
@@ -17346,7 +17365,7 @@
         <v>3.7187999999999999</v>
       </c>
     </row>
-    <row r="191" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B191">
         <v>70618</v>
       </c>
@@ -17393,7 +17412,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="192" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B192">
         <v>70618</v>
       </c>
@@ -17440,7 +17459,7 @@
         <v>2.6440000000000001</v>
       </c>
     </row>
-    <row r="193" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B193">
         <v>70618</v>
       </c>
@@ -17487,7 +17506,7 @@
         <v>5.1562000000000001</v>
       </c>
     </row>
-    <row r="194" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B194">
         <v>70618</v>
       </c>
@@ -17534,7 +17553,7 @@
         <v>2.0937999999999999</v>
       </c>
     </row>
-    <row r="195" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B195">
         <v>70618</v>
       </c>
@@ -17581,7 +17600,7 @@
         <v>3.5312000000000001</v>
       </c>
     </row>
-    <row r="196" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B196">
         <v>70618</v>
       </c>
@@ -17628,7 +17647,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="197" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B197">
         <v>70618</v>
       </c>
@@ -17675,7 +17694,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="198" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B198">
         <v>70618</v>
       </c>
@@ -17722,7 +17741,7 @@
         <v>1.9375</v>
       </c>
     </row>
-    <row r="199" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B199">
         <v>70618</v>
       </c>
@@ -17769,7 +17788,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="200" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B200">
         <v>80618</v>
       </c>
@@ -17816,7 +17835,7 @@
         <v>2.7187999999999999</v>
       </c>
     </row>
-    <row r="201" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B201">
         <v>80618</v>
       </c>
@@ -17863,7 +17882,7 @@
         <v>3.9687999999999999</v>
       </c>
     </row>
-    <row r="202" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B202">
         <v>80618</v>
       </c>
@@ -17910,7 +17929,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="203" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B203">
         <v>80618</v>
       </c>
@@ -17957,7 +17976,7 @@
         <v>2.5937999999999999</v>
       </c>
     </row>
-    <row r="204" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B204">
         <v>80618</v>
       </c>
@@ -18004,7 +18023,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="205" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B205">
         <v>80618</v>
       </c>
@@ -18051,148 +18070,157 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="206" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B206">
+    <row r="206" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B206" s="30">
         <v>251018</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D206">
+      <c r="D206" s="30">
         <v>2</v>
       </c>
-      <c r="E206" s="22" t="s">
+      <c r="E206" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="U206" s="22">
+      <c r="U206" s="30">
         <v>1.2152690863579474</v>
       </c>
-      <c r="V206" s="22">
+      <c r="V206" s="30">
         <v>5.375</v>
       </c>
-      <c r="W206" s="22">
+      <c r="W206" s="30">
         <v>78.697916666666657</v>
       </c>
-      <c r="X206" s="22">
+      <c r="X206" s="30">
         <v>-63.671875</v>
       </c>
-      <c r="Y206" s="22">
+      <c r="Y206" s="30">
         <v>27.869647994896596</v>
       </c>
-      <c r="Z206" s="22">
+      <c r="Z206" s="30">
         <v>11</v>
       </c>
-      <c r="AA206" s="22">
+      <c r="AA206" s="30">
         <v>100.640625</v>
       </c>
-      <c r="AB206" s="22">
+      <c r="AB206" s="30">
         <v>1.1500702911890528</v>
       </c>
-      <c r="AC206" s="22">
+      <c r="AC206" s="30">
         <v>3.125</v>
       </c>
-      <c r="AE206" s="22">
+      <c r="AE206" s="30">
         <v>18.333333333333336</v>
       </c>
-      <c r="AF206" s="22">
+      <c r="AF206" s="30">
         <v>4.2187999999999999</v>
       </c>
     </row>
-    <row r="207" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B207">
+    <row r="207" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B207" s="30">
         <v>251018</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D207">
+      <c r="D207" s="30">
         <v>2</v>
       </c>
-      <c r="E207" s="22" t="s">
+      <c r="E207" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="U207" s="22">
+      <c r="U207" s="30">
         <v>1.1186440677966101</v>
       </c>
-      <c r="V207" s="22">
+      <c r="V207" s="30">
         <v>2.625</v>
       </c>
-      <c r="W207" s="22">
+      <c r="W207" s="30">
         <v>73.802083333333329</v>
       </c>
-      <c r="X207" s="22">
+      <c r="X207" s="30">
         <v>-67.140625</v>
       </c>
-      <c r="Y207" s="22">
+      <c r="Y207" s="30">
         <v>112.30166439348518</v>
       </c>
-      <c r="Z207" s="22">
+      <c r="Z207" s="30">
         <v>7</v>
       </c>
-      <c r="AA207" s="22">
+      <c r="AA207" s="30">
         <v>105.265625</v>
       </c>
-      <c r="AB207" s="22">
+      <c r="AB207" s="30">
         <v>1.0540531448269519</v>
       </c>
-      <c r="AC207" s="22">
+      <c r="AC207" s="30">
         <v>2.40625</v>
       </c>
-      <c r="AE207" s="22">
+      <c r="AE207" s="30">
         <v>11.666666666666668</v>
       </c>
-      <c r="AF207" s="22">
+      <c r="AF207" s="30">
         <v>2.0312000000000001</v>
       </c>
     </row>
-    <row r="208" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B208">
+    <row r="208" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B208" s="30">
         <v>251018</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D208">
+      <c r="D208" s="30">
         <v>2</v>
       </c>
-      <c r="E208" s="22" t="s">
+      <c r="E208" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="U208" s="22">
+      <c r="U208" s="30">
         <v>1.0717749757516974</v>
       </c>
-      <c r="V208" s="22">
+      <c r="V208" s="30">
         <v>2.3125</v>
       </c>
-      <c r="W208" s="22">
+      <c r="W208" s="30">
         <v>104.21874999999999</v>
       </c>
-      <c r="X208" s="22">
+      <c r="X208" s="30">
         <v>-75.203125</v>
       </c>
-      <c r="Y208" s="22">
+      <c r="Y208" s="30">
         <v>47.975891792519235</v>
       </c>
-      <c r="Z208" s="22">
+      <c r="Z208" s="30">
         <v>25</v>
       </c>
-      <c r="AA208" s="22">
+      <c r="AA208" s="30">
         <v>116.078125</v>
       </c>
-      <c r="AB208" s="22">
+      <c r="AB208" s="30">
         <v>1.0647968517550623</v>
       </c>
-      <c r="AC208" s="22">
+      <c r="AC208" s="30">
         <v>1.5</v>
       </c>
-      <c r="AE208" s="22">
+      <c r="AE208" s="30">
         <v>25</v>
       </c>
-      <c r="AF208" s="22">
+      <c r="AF208" s="30">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="209" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B209">
         <v>261018</v>
       </c>
@@ -18205,6 +18233,51 @@
       <c r="E209" s="22" t="s">
         <v>45</v>
       </c>
+      <c r="F209">
+        <v>414.041</v>
+      </c>
+      <c r="G209">
+        <v>259.35399999999998</v>
+      </c>
+      <c r="H209">
+        <v>7.08</v>
+      </c>
+      <c r="I209">
+        <v>52.914000000000001</v>
+      </c>
+      <c r="J209">
+        <v>161.73099999999999</v>
+      </c>
+      <c r="K209">
+        <v>4.0759999999999996</v>
+      </c>
+      <c r="L209">
+        <v>11.571</v>
+      </c>
+      <c r="M209">
+        <v>196.845</v>
+      </c>
+      <c r="N209">
+        <v>67.869</v>
+      </c>
+      <c r="O209">
+        <v>5</v>
+      </c>
+      <c r="P209">
+        <v>106.378</v>
+      </c>
+      <c r="Q209">
+        <v>113.18</v>
+      </c>
+      <c r="R209">
+        <v>32.945999999999998</v>
+      </c>
+      <c r="S209">
+        <v>4</v>
+      </c>
+      <c r="T209">
+        <v>9</v>
+      </c>
       <c r="U209">
         <v>1.1413043478260869</v>
       </c>
@@ -18239,7 +18312,7 @@
         <v>3.8125</v>
       </c>
     </row>
-    <row r="210" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B210">
         <v>261018</v>
       </c>
@@ -18252,6 +18325,51 @@
       <c r="E210" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F210">
+        <v>443.61500000000001</v>
+      </c>
+      <c r="G210">
+        <v>313.976</v>
+      </c>
+      <c r="H210">
+        <v>25.640999999999998</v>
+      </c>
+      <c r="I210">
+        <v>51.963000000000001</v>
+      </c>
+      <c r="J210">
+        <v>196.66499999999999</v>
+      </c>
+      <c r="K210">
+        <v>3.0329999999999999</v>
+      </c>
+      <c r="L210">
+        <v>10.048999999999999</v>
+      </c>
+      <c r="M210">
+        <v>139.09800000000001</v>
+      </c>
+      <c r="N210">
+        <v>78.587000000000003</v>
+      </c>
+      <c r="O210">
+        <v>5</v>
+      </c>
+      <c r="P210">
+        <v>198.49700000000001</v>
+      </c>
+      <c r="Q210">
+        <v>181.428</v>
+      </c>
+      <c r="R210">
+        <v>28.158000000000001</v>
+      </c>
+      <c r="S210">
+        <v>5</v>
+      </c>
+      <c r="T210">
+        <v>6</v>
+      </c>
       <c r="U210">
         <v>1.1631901840490797</v>
       </c>
@@ -18286,7 +18404,7 @@
         <v>3.4062000000000001</v>
       </c>
     </row>
-    <row r="211" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B211">
         <v>261018</v>
       </c>
@@ -18299,6 +18417,51 @@
       <c r="E211" s="22" t="s">
         <v>31</v>
       </c>
+      <c r="F211">
+        <v>416.31799999999998</v>
+      </c>
+      <c r="G211">
+        <v>221.81899999999999</v>
+      </c>
+      <c r="H211">
+        <v>9.1869999999999994</v>
+      </c>
+      <c r="I211">
+        <v>55.000999999999998</v>
+      </c>
+      <c r="J211">
+        <v>205.72200000000001</v>
+      </c>
+      <c r="K211">
+        <v>4.1749999999999998</v>
+      </c>
+      <c r="L211">
+        <v>12.135</v>
+      </c>
+      <c r="M211">
+        <v>133.119</v>
+      </c>
+      <c r="N211">
+        <v>84.174000000000007</v>
+      </c>
+      <c r="O211">
+        <v>4</v>
+      </c>
+      <c r="P211">
+        <v>154.697</v>
+      </c>
+      <c r="Q211">
+        <v>180.98699999999999</v>
+      </c>
+      <c r="R211">
+        <v>13.093</v>
+      </c>
+      <c r="S211">
+        <v>4</v>
+      </c>
+      <c r="T211">
+        <v>8</v>
+      </c>
       <c r="U211">
         <v>1.1590214067278288</v>
       </c>
@@ -18333,7 +18496,7 @@
         <v>3.6875</v>
       </c>
     </row>
-    <row r="212" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B212">
         <v>261018</v>
       </c>
@@ -18346,6 +18509,51 @@
       <c r="E212" s="22" t="s">
         <v>126</v>
       </c>
+      <c r="F212">
+        <v>440.20499999999998</v>
+      </c>
+      <c r="G212">
+        <v>319.649</v>
+      </c>
+      <c r="H212">
+        <v>10.677</v>
+      </c>
+      <c r="I212">
+        <v>48.277999999999999</v>
+      </c>
+      <c r="J212">
+        <v>161.73099999999999</v>
+      </c>
+      <c r="K212">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="L212">
+        <v>9.1020000000000003</v>
+      </c>
+      <c r="M212">
+        <v>145.59700000000001</v>
+      </c>
+      <c r="N212">
+        <v>105.02800000000001</v>
+      </c>
+      <c r="O212">
+        <v>6</v>
+      </c>
+      <c r="P212">
+        <v>176.32300000000001</v>
+      </c>
+      <c r="Q212">
+        <v>126.265</v>
+      </c>
+      <c r="R212">
+        <v>43.423000000000002</v>
+      </c>
+      <c r="S212">
+        <v>5</v>
+      </c>
+      <c r="T212">
+        <v>4</v>
+      </c>
       <c r="U212">
         <v>1.2628571428571429</v>
       </c>
@@ -18377,7 +18585,7 @@
         <v>9.4062000000000001</v>
       </c>
     </row>
-    <row r="213" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B213">
         <v>220519</v>
       </c>
@@ -18424,7 +18632,7 @@
         <v>8.6861999999999995</v>
       </c>
     </row>
-    <row r="214" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B214">
         <v>220519</v>
       </c>
@@ -18468,7 +18676,7 @@
         <v>4.0620000000000003</v>
       </c>
     </row>
-    <row r="215" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B215">
         <v>220519</v>
       </c>
@@ -18515,7 +18723,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="216" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B216">
         <v>220519</v>
       </c>
@@ -18562,7 +18770,7 @@
         <v>5.1875</v>
       </c>
     </row>
-    <row r="217" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B217">
         <v>40918</v>
       </c>
@@ -18606,7 +18814,7 @@
         <v>4.5320999999999998</v>
       </c>
     </row>
-    <row r="218" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B218">
         <v>40918</v>
       </c>
@@ -18650,54 +18858,57 @@
         <v>3.3125</v>
       </c>
     </row>
-    <row r="219" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B219">
+    <row r="219" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B219" s="30">
         <v>11018</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D219">
+      <c r="D219" s="30">
         <v>2</v>
       </c>
-      <c r="E219" s="22" t="s">
+      <c r="E219" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="U219">
+      <c r="U219" s="30">
         <v>1.1166464155528555</v>
       </c>
-      <c r="V219">
+      <c r="V219" s="30">
         <v>3</v>
       </c>
-      <c r="W219">
+      <c r="W219" s="30">
         <v>83.406249999999972</v>
       </c>
-      <c r="X219">
+      <c r="X219" s="30">
         <v>-65.759375000000006</v>
       </c>
-      <c r="Y219">
+      <c r="Y219" s="30">
         <v>20.380017688410859</v>
       </c>
-      <c r="Z219" s="22">
+      <c r="Z219" s="30">
         <v>17</v>
       </c>
-      <c r="AA219">
+      <c r="AA219" s="30">
         <v>112.94687500000001</v>
       </c>
-      <c r="AB219">
+      <c r="AB219" s="30">
         <v>1.0032131299494864</v>
       </c>
-      <c r="AC219">
+      <c r="AC219" s="30">
         <v>2.25</v>
       </c>
-      <c r="AE219">
+      <c r="AE219" s="30">
         <v>28.333333333333336</v>
       </c>
-      <c r="AF219" s="22">
+      <c r="AF219" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B220">
         <v>11018</v>
       </c>
@@ -18710,6 +18921,51 @@
       <c r="E220" s="22" t="s">
         <v>35</v>
       </c>
+      <c r="F220">
+        <v>385.31</v>
+      </c>
+      <c r="G220">
+        <v>185.31200000000001</v>
+      </c>
+      <c r="H220">
+        <v>15.185</v>
+      </c>
+      <c r="I220">
+        <v>44.673000000000002</v>
+      </c>
+      <c r="J220">
+        <v>139.946</v>
+      </c>
+      <c r="K220">
+        <v>2.7280000000000002</v>
+      </c>
+      <c r="L220">
+        <v>13.61</v>
+      </c>
+      <c r="M220">
+        <v>148.85599999999999</v>
+      </c>
+      <c r="N220">
+        <v>116.83</v>
+      </c>
+      <c r="O220">
+        <v>6</v>
+      </c>
+      <c r="P220">
+        <v>243.947</v>
+      </c>
+      <c r="Q220">
+        <v>185.489</v>
+      </c>
+      <c r="R220">
+        <v>42.658999999999999</v>
+      </c>
+      <c r="S220">
+        <v>4</v>
+      </c>
+      <c r="T220">
+        <v>6</v>
+      </c>
       <c r="U220">
         <v>1.2399497487437185</v>
       </c>
@@ -18744,51 +19000,54 @@
         <v>5.9687999999999999</v>
       </c>
     </row>
-    <row r="221" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B221">
+    <row r="221" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="B221" s="30">
         <v>21018</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D221">
+      <c r="D221" s="30">
         <v>2</v>
       </c>
-      <c r="E221" s="22" t="s">
+      <c r="E221" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="U221" s="22">
+      <c r="U221" s="30">
         <v>1.058457711442786</v>
       </c>
-      <c r="V221" s="22">
+      <c r="V221" s="30">
         <v>1.46875</v>
       </c>
-      <c r="W221" s="22">
+      <c r="W221" s="30">
         <v>80.968750000000014</v>
       </c>
-      <c r="X221" s="22">
+      <c r="X221" s="30">
         <v>-67.240624999999994</v>
       </c>
-      <c r="Y221" s="22">
+      <c r="Y221" s="30">
         <v>103.98393335187315</v>
       </c>
-      <c r="Z221" s="22">
+      <c r="Z221" s="30">
         <v>14</v>
       </c>
-      <c r="AA221" s="22">
+      <c r="AA221" s="30">
         <v>110.74062499999999</v>
       </c>
-      <c r="AB221" s="22">
+      <c r="AB221" s="30">
         <v>1.0290353798435561</v>
       </c>
-      <c r="AE221" s="22">
+      <c r="AE221" s="30">
         <v>23.333333333333336</v>
       </c>
-      <c r="AF221" s="22">
+      <c r="AF221" s="30">
         <v>0.21875</v>
       </c>
     </row>
-    <row r="222" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B222">
         <v>21018</v>
       </c>
@@ -18801,6 +19060,51 @@
       <c r="E222" s="22" t="s">
         <v>32</v>
       </c>
+      <c r="F222">
+        <v>342.95400000000001</v>
+      </c>
+      <c r="G222">
+        <v>200.45099999999999</v>
+      </c>
+      <c r="H222">
+        <v>11.521000000000001</v>
+      </c>
+      <c r="I222">
+        <v>40.996000000000002</v>
+      </c>
+      <c r="J222">
+        <v>113.411</v>
+      </c>
+      <c r="K222">
+        <v>1.744</v>
+      </c>
+      <c r="L222">
+        <v>9.6910000000000007</v>
+      </c>
+      <c r="M222">
+        <v>113.45699999999999</v>
+      </c>
+      <c r="N222">
+        <v>64.356999999999999</v>
+      </c>
+      <c r="O222">
+        <v>5</v>
+      </c>
+      <c r="P222">
+        <v>120.851</v>
+      </c>
+      <c r="Q222">
+        <v>133.298</v>
+      </c>
+      <c r="R222">
+        <v>27.148</v>
+      </c>
+      <c r="S222">
+        <v>4</v>
+      </c>
+      <c r="T222">
+        <v>3</v>
+      </c>
       <c r="U222" s="22">
         <v>1.1147036181678214</v>
       </c>
@@ -18835,15 +19139,63 @@
         <v>1.1875</v>
       </c>
     </row>
-    <row r="223" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B223">
         <v>270319</v>
       </c>
       <c r="C223" t="s">
         <v>107</v>
       </c>
+      <c r="D223" s="30">
+        <v>2</v>
+      </c>
       <c r="E223" s="22" t="s">
         <v>28</v>
+      </c>
+      <c r="F223">
+        <v>451.137</v>
+      </c>
+      <c r="G223">
+        <v>325.56900000000002</v>
+      </c>
+      <c r="H223">
+        <v>12.055</v>
+      </c>
+      <c r="I223">
+        <v>48.258000000000003</v>
+      </c>
+      <c r="J223">
+        <v>159.155</v>
+      </c>
+      <c r="K223">
+        <v>2.3690000000000002</v>
+      </c>
+      <c r="L223">
+        <v>11.589</v>
+      </c>
+      <c r="M223">
+        <v>167.91399999999999</v>
+      </c>
+      <c r="N223">
+        <v>92.045000000000002</v>
+      </c>
+      <c r="O223">
+        <v>4</v>
+      </c>
+      <c r="P223">
+        <v>186.37100000000001</v>
+      </c>
+      <c r="Q223">
+        <v>124.443</v>
+      </c>
+      <c r="R223">
+        <v>77.769000000000005</v>
+      </c>
+      <c r="S223">
+        <v>4</v>
+      </c>
+      <c r="T223">
+        <v>4</v>
       </c>
       <c r="U223" s="22">
         <v>1.1842496285289748</v>
@@ -18880,16 +19232,64 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="224" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B224">
         <v>270319</v>
       </c>
       <c r="C224" t="s">
         <v>107</v>
       </c>
+      <c r="D224">
+        <v>3</v>
+      </c>
       <c r="E224" s="22" t="s">
         <v>47</v>
       </c>
+      <c r="F224">
+        <v>488.06900000000002</v>
+      </c>
+      <c r="G224">
+        <v>309.09100000000001</v>
+      </c>
+      <c r="H224">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="I224">
+        <v>49.122</v>
+      </c>
+      <c r="J224">
+        <v>143.66</v>
+      </c>
+      <c r="K224">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="L224">
+        <v>13.068</v>
+      </c>
+      <c r="M224">
+        <v>89.772999999999996</v>
+      </c>
+      <c r="N224">
+        <v>81.501000000000005</v>
+      </c>
+      <c r="O224">
+        <v>4</v>
+      </c>
+      <c r="P224">
+        <v>146.59100000000001</v>
+      </c>
+      <c r="Q224">
+        <v>112.501</v>
+      </c>
+      <c r="R224">
+        <v>38.253999999999998</v>
+      </c>
+      <c r="S224">
+        <v>5</v>
+      </c>
+      <c r="T224">
+        <v>4</v>
+      </c>
       <c r="U224" s="22">
         <v>1.1585106382978723</v>
       </c>
@@ -18924,15 +19324,63 @@
         <v>4.1224999999999996</v>
       </c>
     </row>
-    <row r="225" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B225">
         <v>270319</v>
       </c>
       <c r="C225" t="s">
         <v>107</v>
       </c>
+      <c r="D225" s="30">
+        <v>3</v>
+      </c>
       <c r="E225" s="22" t="s">
         <v>35</v>
+      </c>
+      <c r="F225">
+        <v>553.15</v>
+      </c>
+      <c r="G225">
+        <v>388.49599999999998</v>
+      </c>
+      <c r="H225">
+        <v>46.121000000000002</v>
+      </c>
+      <c r="I225">
+        <v>43.274000000000001</v>
+      </c>
+      <c r="J225">
+        <v>115.51900000000001</v>
+      </c>
+      <c r="K225">
+        <v>1.8959999999999999</v>
+      </c>
+      <c r="L225">
+        <v>15.782</v>
+      </c>
+      <c r="M225">
+        <v>95.480999999999995</v>
+      </c>
+      <c r="N225">
+        <v>61.338000000000001</v>
+      </c>
+      <c r="O225">
+        <v>5</v>
+      </c>
+      <c r="P225">
+        <v>185.809</v>
+      </c>
+      <c r="Q225">
+        <v>165.83199999999999</v>
+      </c>
+      <c r="R225">
+        <v>26.248999999999999</v>
+      </c>
+      <c r="S225">
+        <v>2</v>
+      </c>
+      <c r="T225">
+        <v>0</v>
       </c>
       <c r="U225" s="22">
         <v>1.0929203539823009</v>
@@ -18966,7 +19414,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="226" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B226">
         <v>270320</v>
       </c>
@@ -19028,13 +19476,13 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
@@ -19053,7 +19501,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -19068,7 +19516,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
@@ -19087,7 +19535,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -19104,7 +19552,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -19117,7 +19565,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>21</v>
       </c>
@@ -19136,7 +19584,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -19155,7 +19603,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -19174,7 +19622,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -19193,7 +19641,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -19212,7 +19660,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -19231,7 +19679,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
@@ -19252,7 +19700,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -19271,7 +19719,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K20" s="8" t="s">
         <v>16</v>
       </c>
@@ -19282,7 +19730,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -19296,43 +19744,43 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>

</xml_diff>